<commit_message>
bs_feom_notes api route build plus NOTESTOLALL folder
</commit_message>
<xml_diff>
--- a/notestoALL/outputbs_Sheet.xlsx
+++ b/notestoALL/outputbs_Sheet.xlsx
@@ -556,8 +556,16 @@
           <t>2</t>
         </is>
       </c>
-      <c r="C6" s="10" t="inlineStr"/>
-      <c r="D6" s="10" t="inlineStr"/>
+      <c r="C6" s="10" t="inlineStr">
+        <is>
+          <t>204.86</t>
+        </is>
+      </c>
+      <c r="D6" s="10" t="inlineStr">
+        <is>
+          <t>2,046.90</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="8" t="inlineStr">
@@ -571,13 +579,25 @@
         </is>
       </c>
       <c r="C7" s="10" t="inlineStr"/>
-      <c r="D7" s="10" t="inlineStr"/>
+      <c r="D7" s="10" t="inlineStr">
+        <is>
+          <t>9,958.15</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="7" t="inlineStr"/>
       <c r="B8" s="9" t="inlineStr"/>
-      <c r="C8" s="11" t="inlineStr"/>
-      <c r="D8" s="11" t="inlineStr"/>
+      <c r="C8" s="11" t="inlineStr">
+        <is>
+          <t>204.86</t>
+        </is>
+      </c>
+      <c r="D8" s="11" t="inlineStr">
+        <is>
+          <t>12,005.06</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="7" t="inlineStr">
@@ -601,7 +621,11 @@
         </is>
       </c>
       <c r="C10" s="10" t="inlineStr"/>
-      <c r="D10" s="10" t="inlineStr"/>
+      <c r="D10" s="10" t="inlineStr">
+        <is>
+          <t>914.46</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="8" t="inlineStr">
@@ -615,13 +639,21 @@
         </is>
       </c>
       <c r="C11" s="10" t="inlineStr"/>
-      <c r="D11" s="10" t="inlineStr"/>
+      <c r="D11" s="10" t="inlineStr">
+        <is>
+          <t>49.00</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="7" t="inlineStr"/>
       <c r="B12" s="9" t="inlineStr"/>
       <c r="C12" s="11" t="inlineStr"/>
-      <c r="D12" s="11" t="inlineStr"/>
+      <c r="D12" s="11" t="inlineStr">
+        <is>
+          <t>963.46</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="7" t="inlineStr">
@@ -644,8 +676,16 @@
           <t>6</t>
         </is>
       </c>
-      <c r="C14" s="10" t="inlineStr"/>
-      <c r="D14" s="10" t="inlineStr"/>
+      <c r="C14" s="10" t="inlineStr">
+        <is>
+          <t>491.39</t>
+        </is>
+      </c>
+      <c r="D14" s="10" t="inlineStr">
+        <is>
+          <t>104.23</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="8" t="inlineStr">
@@ -659,7 +699,11 @@
         </is>
       </c>
       <c r="C15" s="10" t="inlineStr"/>
-      <c r="D15" s="10" t="inlineStr"/>
+      <c r="D15" s="10" t="inlineStr">
+        <is>
+          <t>125.35</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="8" t="inlineStr">
@@ -673,13 +717,25 @@
         </is>
       </c>
       <c r="C16" s="10" t="inlineStr"/>
-      <c r="D16" s="10" t="inlineStr"/>
+      <c r="D16" s="10" t="inlineStr">
+        <is>
+          <t>179.27</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="7" t="inlineStr"/>
       <c r="B17" s="9" t="inlineStr"/>
-      <c r="C17" s="11" t="inlineStr"/>
-      <c r="D17" s="11" t="inlineStr"/>
+      <c r="C17" s="11" t="inlineStr">
+        <is>
+          <t>491.39</t>
+        </is>
+      </c>
+      <c r="D17" s="11" t="inlineStr">
+        <is>
+          <t>408.85</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="5" t="inlineStr">
@@ -688,8 +744,16 @@
         </is>
       </c>
       <c r="B18" s="9" t="inlineStr"/>
-      <c r="C18" s="11" t="inlineStr"/>
-      <c r="D18" s="11" t="inlineStr"/>
+      <c r="C18" s="11" t="inlineStr">
+        <is>
+          <t>696.25</t>
+        </is>
+      </c>
+      <c r="D18" s="11" t="inlineStr">
+        <is>
+          <t>13,377.37</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="inlineStr">
@@ -766,13 +830,21 @@
           <t>10</t>
         </is>
       </c>
-      <c r="C25" s="10" t="inlineStr"/>
+      <c r="C25" s="10" t="inlineStr">
+        <is>
+          <t>0.60</t>
+        </is>
+      </c>
       <c r="D25" s="10" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="7" t="inlineStr"/>
       <c r="B26" s="9" t="inlineStr"/>
-      <c r="C26" s="11" t="inlineStr"/>
+      <c r="C26" s="11" t="inlineStr">
+        <is>
+          <t>0.60</t>
+        </is>
+      </c>
       <c r="D26" s="11" t="inlineStr"/>
     </row>
     <row r="27">
@@ -898,7 +970,7 @@
       <c r="B34" s="9" t="inlineStr"/>
       <c r="C34" s="11" t="inlineStr">
         <is>
-          <t>3,884.46</t>
+          <t>3,885.06</t>
         </is>
       </c>
       <c r="D34" s="11" t="inlineStr">

</xml_diff>